<commit_message>
Updated on 02-26-2024 at 23:24
</commit_message>
<xml_diff>
--- a/experiment_2/output/mean_per_day_re.xlsx
+++ b/experiment_2/output/mean_per_day_re.xlsx
@@ -505,34 +505,34 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.042965</v>
+        <v>0.047138</v>
       </c>
       <c r="C3" t="n">
-        <v>0.123241</v>
+        <v>0.144842</v>
       </c>
       <c r="D3" t="n">
-        <v>0.200328</v>
+        <v>0.250829</v>
       </c>
       <c r="E3" t="n">
-        <v>0.314857</v>
+        <v>0.400816</v>
       </c>
       <c r="F3" t="n">
-        <v>0.503655</v>
+        <v>0.63916</v>
       </c>
       <c r="G3" t="n">
-        <v>0.715079</v>
+        <v>0.912927</v>
       </c>
       <c r="H3" t="n">
-        <v>1.032306</v>
+        <v>1.319782</v>
       </c>
       <c r="I3" t="n">
-        <v>1.343534</v>
+        <v>1.746352</v>
       </c>
       <c r="J3" t="n">
-        <v>1.668063</v>
+        <v>2.188998</v>
       </c>
       <c r="K3" t="n">
-        <v>2.065336</v>
+        <v>2.737404</v>
       </c>
     </row>
     <row r="4">
@@ -540,34 +540,34 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.036773</v>
+        <v>0.037583</v>
       </c>
       <c r="C4" t="n">
-        <v>0.084123</v>
+        <v>0.096954</v>
       </c>
       <c r="D4" t="n">
-        <v>0.147368</v>
+        <v>0.155449</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2362</v>
+        <v>0.240405</v>
       </c>
       <c r="F4" t="n">
-        <v>0.37125</v>
+        <v>0.384114</v>
       </c>
       <c r="G4" t="n">
-        <v>0.513192</v>
+        <v>0.5403019999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>0.724287</v>
+        <v>0.780771</v>
       </c>
       <c r="I4" t="n">
-        <v>0.89667</v>
+        <v>1.002947</v>
       </c>
       <c r="J4" t="n">
-        <v>1.099896</v>
+        <v>1.229073</v>
       </c>
       <c r="K4" t="n">
-        <v>1.340487</v>
+        <v>1.502442</v>
       </c>
     </row>
     <row r="5">
@@ -575,34 +575,34 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.032479</v>
+        <v>0.032457</v>
       </c>
       <c r="C5" t="n">
-        <v>0.076747</v>
+        <v>0.073694</v>
       </c>
       <c r="D5" t="n">
-        <v>0.09697500000000001</v>
+        <v>0.117879</v>
       </c>
       <c r="E5" t="n">
-        <v>0.146652</v>
+        <v>0.187573</v>
       </c>
       <c r="F5" t="n">
-        <v>0.239589</v>
+        <v>0.296455</v>
       </c>
       <c r="G5" t="n">
-        <v>0.338938</v>
+        <v>0.415213</v>
       </c>
       <c r="H5" t="n">
-        <v>0.480119</v>
+        <v>0.582352</v>
       </c>
       <c r="I5" t="n">
-        <v>0.572735</v>
+        <v>0.706772</v>
       </c>
       <c r="J5" t="n">
-        <v>0.696315</v>
+        <v>0.862469</v>
       </c>
       <c r="K5" t="n">
-        <v>0.827935</v>
+        <v>1.034064</v>
       </c>
     </row>
     <row r="6">
@@ -610,34 +610,34 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.033933</v>
+        <v>0.031291</v>
       </c>
       <c r="C6" t="n">
-        <v>0.07750600000000001</v>
+        <v>0.077972</v>
       </c>
       <c r="D6" t="n">
-        <v>0.09829</v>
+        <v>0.095669</v>
       </c>
       <c r="E6" t="n">
-        <v>0.132623</v>
+        <v>0.126333</v>
       </c>
       <c r="F6" t="n">
-        <v>0.190049</v>
+        <v>0.203711</v>
       </c>
       <c r="G6" t="n">
-        <v>0.265703</v>
+        <v>0.287863</v>
       </c>
       <c r="H6" t="n">
-        <v>0.380255</v>
+        <v>0.411415</v>
       </c>
       <c r="I6" t="n">
-        <v>0.476589</v>
+        <v>0.502936</v>
       </c>
       <c r="J6" t="n">
-        <v>0.559561</v>
+        <v>0.59468</v>
       </c>
       <c r="K6" t="n">
-        <v>0.651508</v>
+        <v>0.690595</v>
       </c>
     </row>
     <row r="7">
@@ -645,34 +645,34 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.031134</v>
+        <v>0.034444</v>
       </c>
       <c r="C7" t="n">
-        <v>0.06808</v>
+        <v>0.07885300000000001</v>
       </c>
       <c r="D7" t="n">
-        <v>0.073448</v>
+        <v>0.100539</v>
       </c>
       <c r="E7" t="n">
-        <v>0.096784</v>
+        <v>0.135941</v>
       </c>
       <c r="F7" t="n">
-        <v>0.129393</v>
+        <v>0.194621</v>
       </c>
       <c r="G7" t="n">
-        <v>0.162632</v>
+        <v>0.271772</v>
       </c>
       <c r="H7" t="n">
-        <v>0.216748</v>
+        <v>0.38813</v>
       </c>
       <c r="I7" t="n">
-        <v>0.272334</v>
+        <v>0.483397</v>
       </c>
       <c r="J7" t="n">
-        <v>0.311283</v>
+        <v>0.568499</v>
       </c>
       <c r="K7" t="n">
-        <v>0.348593</v>
+        <v>0.660315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>